<commit_message>
Use locale code instead
</commit_message>
<xml_diff>
--- a/home/tests/import-export-data/ordered_content.xlsx
+++ b/home/tests/import-export-data/ordered_content.xlsx
@@ -69,7 +69,7 @@
     <t>test-set</t>
   </si>
   <si>
-    <t>English</t>
+    <t>en</t>
   </si>
 </sst>
 </file>
@@ -86,7 +86,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -359,10 +358,10 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -388,7 +387,7 @@
       <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="2" t="s">

</xml_diff>